<commit_message>
Update sfa in files
</commit_message>
<xml_diff>
--- a/三阶段各省各年份碳排放效率对比表.xlsx
+++ b/三阶段各省各年份碳排放效率对比表.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikezhu/Desktop/碳排放数据/dea_process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{28EBDC40-8FE7-4B4D-9D64-C9384E882CBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0B34F0D0-1D60-D540-8C1C-8CE8EC967C6D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1160" windowWidth="28800" windowHeight="16460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Carbon Emission" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1124,7 +1124,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8EEB5D6B-A7B9-254B-AF1C-437B68C5AA71}</c15:txfldGUID>
+                      <c15:txfldGUID>{DE47F0EE-4B32-2043-B54B-F58FCEFF4278}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$35</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1165,7 +1165,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{277EBAF2-326F-1F49-9407-CC8D36F9A94C}</c15:txfldGUID>
+                      <c15:txfldGUID>{EB2FC683-D09F-5645-8403-B48004F64F70}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$36</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1206,7 +1206,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3FEC30CE-9110-C946-8FF9-AFD2EE33BAD2}</c15:txfldGUID>
+                      <c15:txfldGUID>{CB72B63D-FB4B-644A-8EF1-7BF35577BA80}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$37</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1247,7 +1247,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E4D0B688-EDE3-0A4D-9131-526FBD073A8F}</c15:txfldGUID>
+                      <c15:txfldGUID>{A16E7653-9B02-364A-B3A6-01C15644CDA4}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$38</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1288,7 +1288,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2DB7D1F2-AEDD-044E-AC8E-8C77EA57AFF0}</c15:txfldGUID>
+                      <c15:txfldGUID>{A5D41C81-33C4-8245-B0DA-36457C707429}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$39</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1329,7 +1329,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CB239E10-5FD0-7846-93B9-7EB20C450F4F}</c15:txfldGUID>
+                      <c15:txfldGUID>{C04D8D48-DE79-774C-B91D-F696B76DD3E5}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$40</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1370,7 +1370,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2F3C2888-DC83-9948-85D4-F0112DDAABC0}</c15:txfldGUID>
+                      <c15:txfldGUID>{6FEA8470-D434-AB44-B375-32C50443C32A}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$41</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1411,7 +1411,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{338949B9-BB40-2344-AD23-853EAD0FBDB6}</c15:txfldGUID>
+                      <c15:txfldGUID>{F0DB950C-4B81-D34F-9C68-619899177CFF}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$42</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1452,7 +1452,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8D94BC87-58D0-5141-8094-F6CF58199EF5}</c15:txfldGUID>
+                      <c15:txfldGUID>{1FD33399-F997-434D-8FFF-371FCA7DA571}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$43</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1493,7 +1493,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C6CF2F76-E9DD-6D43-A0AC-32588D335D7A}</c15:txfldGUID>
+                      <c15:txfldGUID>{A471F7C9-0B0D-FC4F-B8DF-DE4301241121}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$44</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1534,7 +1534,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{34E40F7E-0BFC-374A-95C8-26B4438B2492}</c15:txfldGUID>
+                      <c15:txfldGUID>{4271E248-A81C-AC4E-9BDA-CB2668E09E0B}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$45</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1575,7 +1575,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2A43C0E3-612B-E54D-B723-A6F56ECDF8EA}</c15:txfldGUID>
+                      <c15:txfldGUID>{A4803513-4ADF-2C4D-B47A-A7D000F9C484}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$46</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1616,7 +1616,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{011A2A83-A9FC-634F-996E-67E8B06DE91E}</c15:txfldGUID>
+                      <c15:txfldGUID>{30F1E2F7-08C7-CC43-AF0C-FB9B356B52A8}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$47</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1657,7 +1657,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4FEBC862-5637-FD44-BE9A-27B6AF4FCC24}</c15:txfldGUID>
+                      <c15:txfldGUID>{661B5B8A-CFFF-3640-99C9-2E5F738BC716}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$48</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1698,7 +1698,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AAEA3BD8-65D7-2B4C-965B-2446AF8F92BF}</c15:txfldGUID>
+                      <c15:txfldGUID>{9A0AE114-E67E-1F4E-83FB-E9B64AF249B0}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$49</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1739,7 +1739,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D2720920-6DD8-0F46-9AD7-78A4ACE9F61C}</c15:txfldGUID>
+                      <c15:txfldGUID>{77850622-FC81-D545-8B04-45F8A33F3A91}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$50</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1780,7 +1780,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AEC1B1C5-EA6C-E444-90A8-B08B56AB80EC}</c15:txfldGUID>
+                      <c15:txfldGUID>{366B45EA-1309-C84E-87B9-F39576DC0118}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$51</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1821,7 +1821,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1B903B50-0E36-474F-A86C-4030D96499D4}</c15:txfldGUID>
+                      <c15:txfldGUID>{0E88710F-FF5B-3C4D-8BCA-96377FCC2D10}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$52</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1862,7 +1862,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6CF60400-E158-7243-BAF2-1789C536A1BE}</c15:txfldGUID>
+                      <c15:txfldGUID>{BC838F03-DE22-A142-8DFF-694FA2F399EF}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$53</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1903,7 +1903,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1644AF3C-8E22-F045-BF95-EF812DFBEA99}</c15:txfldGUID>
+                      <c15:txfldGUID>{61C2454C-E00E-6846-AA4A-B2B55C48FCD8}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$54</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1944,7 +1944,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4854F7FD-78B4-5D4B-828E-95155E8D23BE}</c15:txfldGUID>
+                      <c15:txfldGUID>{03D39D5E-EB34-0A41-96D6-DEA51F629D29}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$55</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1985,7 +1985,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{31DE10C2-C4AD-1F4D-B8B5-789C37CB981E}</c15:txfldGUID>
+                      <c15:txfldGUID>{E98FFA55-D924-E345-BB9F-0133D810875D}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$56</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2026,7 +2026,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E2A97C3C-C4C6-3D4A-8BE9-9E28690FE2EE}</c15:txfldGUID>
+                      <c15:txfldGUID>{3DD8B4E2-C5EF-E347-BFBA-C3767AAB2FD7}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$57</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2067,7 +2067,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EE63DD94-FC61-D54C-BFF6-D95C70DA255C}</c15:txfldGUID>
+                      <c15:txfldGUID>{C98DD0A7-5D37-A547-AF7A-553C8DCD0CCA}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$58</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2108,7 +2108,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B50D61CE-8920-7949-A6F0-D12B52E03761}</c15:txfldGUID>
+                      <c15:txfldGUID>{F90F37C9-C1E3-B347-A83E-C1843D981763}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$59</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2149,7 +2149,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{43BD3ABE-EE84-024E-AA7B-4A8878834BEA}</c15:txfldGUID>
+                      <c15:txfldGUID>{96687B42-CF3C-B146-9CD9-F61673B0C2F6}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$60</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2190,7 +2190,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{576BB4FC-3817-A741-89A4-E92AE6780605}</c15:txfldGUID>
+                      <c15:txfldGUID>{CA725189-D14B-2140-B5C7-1032326CD434}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$61</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2231,7 +2231,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{92C3AB1E-4D75-AE4A-875B-8558969D6265}</c15:txfldGUID>
+                      <c15:txfldGUID>{C1914029-9773-0D43-AD6B-B269EA6FCC9D}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$62</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2272,7 +2272,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B24CD7C9-D322-2840-AE24-9F342E72ECE4}</c15:txfldGUID>
+                      <c15:txfldGUID>{9040BE58-FCB0-0642-9728-323BD7A68427}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$63</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2313,7 +2313,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{09BDB941-0CF1-084E-915D-D5390C48428A}</c15:txfldGUID>
+                      <c15:txfldGUID>{C1C6BC1A-F2A3-DC44-ADB2-663BD06B6443}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$64</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2354,7 +2354,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4EC13EA8-0246-7540-B0C5-CD7EDE135BB9}</c15:txfldGUID>
+                      <c15:txfldGUID>{6BC1AC71-7486-D04D-A782-2B861967C833}</c15:txfldGUID>
                       <c15:f>[1]Sheet1!$A$65</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2872,37 +2872,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65%"/>
-                  <a:lumOff val="35%"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -4055,7 +4025,7 @@
         <c:dLbls>
           <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -4079,8 +4049,13 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15%"/>
+                <a:lumOff val="85%"/>
+              </a:schemeClr>
+            </a:solidFill>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -4117,12 +4092,53 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1679974992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -5984,264 +6000,6 @@
           <cell r="M33" t="str">
             <v>2006年</v>
           </cell>
-          <cell r="N33" t="str">
-            <v>2007年</v>
-          </cell>
-          <cell r="O33" t="str">
-            <v>2008年</v>
-          </cell>
-          <cell r="P33" t="str">
-            <v>2009年</v>
-          </cell>
-          <cell r="Q33" t="str">
-            <v>2010年</v>
-          </cell>
-          <cell r="R33" t="str">
-            <v>2011年</v>
-          </cell>
-          <cell r="S33" t="str">
-            <v>2012年</v>
-          </cell>
-          <cell r="T33" t="str">
-            <v>2013年</v>
-          </cell>
-          <cell r="U33" t="str">
-            <v>2014年</v>
-          </cell>
-          <cell r="V33" t="str">
-            <v>2015年</v>
-          </cell>
-          <cell r="W33" t="str">
-            <v>2016年</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>北京市</v>
-          </cell>
-          <cell r="M35">
-            <v>13</v>
-          </cell>
-          <cell r="N35">
-            <v>13</v>
-          </cell>
-          <cell r="O35">
-            <v>13</v>
-          </cell>
-          <cell r="P35">
-            <v>14</v>
-          </cell>
-          <cell r="Q35">
-            <v>13</v>
-          </cell>
-          <cell r="R35">
-            <v>14</v>
-          </cell>
-          <cell r="S35">
-            <v>14</v>
-          </cell>
-          <cell r="T35">
-            <v>14</v>
-          </cell>
-          <cell r="U35">
-            <v>14</v>
-          </cell>
-          <cell r="V35">
-            <v>14</v>
-          </cell>
-          <cell r="W35">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>天津市</v>
-          </cell>
-          <cell r="M36">
-            <v>23</v>
-          </cell>
-          <cell r="N36">
-            <v>23</v>
-          </cell>
-          <cell r="O36">
-            <v>22</v>
-          </cell>
-          <cell r="P36">
-            <v>22</v>
-          </cell>
-          <cell r="Q36">
-            <v>21</v>
-          </cell>
-          <cell r="R36">
-            <v>21</v>
-          </cell>
-          <cell r="S36">
-            <v>21</v>
-          </cell>
-          <cell r="T36">
-            <v>20</v>
-          </cell>
-          <cell r="U36">
-            <v>20</v>
-          </cell>
-          <cell r="V36">
-            <v>21</v>
-          </cell>
-          <cell r="W36">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>上海市</v>
-          </cell>
-          <cell r="M43">
-            <v>9</v>
-          </cell>
-          <cell r="N43">
-            <v>8</v>
-          </cell>
-          <cell r="O43">
-            <v>9</v>
-          </cell>
-          <cell r="P43">
-            <v>11</v>
-          </cell>
-          <cell r="Q43">
-            <v>11</v>
-          </cell>
-          <cell r="R43">
-            <v>11</v>
-          </cell>
-          <cell r="S43">
-            <v>12</v>
-          </cell>
-          <cell r="T43">
-            <v>12</v>
-          </cell>
-          <cell r="U43">
-            <v>12</v>
-          </cell>
-          <cell r="V43">
-            <v>13</v>
-          </cell>
-          <cell r="W43">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>湖北省</v>
-          </cell>
-          <cell r="M51">
-            <v>12</v>
-          </cell>
-          <cell r="N51">
-            <v>11</v>
-          </cell>
-          <cell r="O51">
-            <v>11</v>
-          </cell>
-          <cell r="P51">
-            <v>10</v>
-          </cell>
-          <cell r="Q51">
-            <v>10</v>
-          </cell>
-          <cell r="R51">
-            <v>10</v>
-          </cell>
-          <cell r="S51">
-            <v>10</v>
-          </cell>
-          <cell r="T51">
-            <v>10</v>
-          </cell>
-          <cell r="U51">
-            <v>10</v>
-          </cell>
-          <cell r="V51">
-            <v>10</v>
-          </cell>
-          <cell r="W51">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>广东省</v>
-          </cell>
-          <cell r="M53">
-            <v>1</v>
-          </cell>
-          <cell r="N53">
-            <v>1</v>
-          </cell>
-          <cell r="O53">
-            <v>1</v>
-          </cell>
-          <cell r="P53">
-            <v>1</v>
-          </cell>
-          <cell r="Q53">
-            <v>1</v>
-          </cell>
-          <cell r="R53">
-            <v>1</v>
-          </cell>
-          <cell r="S53">
-            <v>1</v>
-          </cell>
-          <cell r="T53">
-            <v>1</v>
-          </cell>
-          <cell r="U53">
-            <v>1</v>
-          </cell>
-          <cell r="V53">
-            <v>1</v>
-          </cell>
-          <cell r="W53">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>重庆市</v>
-          </cell>
-          <cell r="M56">
-            <v>24</v>
-          </cell>
-          <cell r="N56">
-            <v>24</v>
-          </cell>
-          <cell r="O56">
-            <v>24</v>
-          </cell>
-          <cell r="P56">
-            <v>23</v>
-          </cell>
-          <cell r="Q56">
-            <v>23</v>
-          </cell>
-          <cell r="R56">
-            <v>23</v>
-          </cell>
-          <cell r="S56">
-            <v>23</v>
-          </cell>
-          <cell r="T56">
-            <v>21</v>
-          </cell>
-          <cell r="U56">
-            <v>21</v>
-          </cell>
-          <cell r="V56">
-            <v>19</v>
-          </cell>
-          <cell r="W56">
-            <v>18</v>
-          </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
@@ -6249,523 +6007,160 @@
           <cell r="B1" t="str">
             <v>2006年</v>
           </cell>
-          <cell r="C1" t="str">
-            <v>2007年</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>2008年</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>2009年</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>2010年</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>2011年</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>2012年</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>2013年</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>2014年</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>2015年</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>2016年</v>
-          </cell>
         </row>
         <row r="35">
           <cell r="A35" t="str">
             <v>北京市</v>
-          </cell>
-          <cell r="M35">
-            <v>0.30573298181818181</v>
-          </cell>
-          <cell r="N35">
-            <v>82123.545454545456</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36" t="str">
             <v>天津市</v>
           </cell>
-          <cell r="M36">
-            <v>0.20827786000000001</v>
-          </cell>
-          <cell r="N36">
-            <v>80899.090909090912</v>
-          </cell>
         </row>
         <row r="37">
           <cell r="A37" t="str">
             <v>河北省</v>
-          </cell>
-          <cell r="M37">
-            <v>0.48088283454545455</v>
-          </cell>
-          <cell r="N37">
-            <v>31414</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38" t="str">
             <v>山西省</v>
           </cell>
-          <cell r="M38">
-            <v>0.21338889272727277</v>
-          </cell>
-          <cell r="N38">
-            <v>27882.909090909092</v>
-          </cell>
         </row>
         <row r="39">
           <cell r="A39" t="str">
             <v>内蒙古自治区</v>
-          </cell>
-          <cell r="M39">
-            <v>0.25181521363636361</v>
-          </cell>
-          <cell r="N39">
-            <v>52038.727272727272</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40" t="str">
             <v>辽宁省</v>
           </cell>
-          <cell r="M40">
-            <v>0.42879501909090911</v>
-          </cell>
-          <cell r="N40">
-            <v>46168.454545454544</v>
-          </cell>
         </row>
         <row r="41">
           <cell r="A41" t="str">
             <v>吉林省</v>
-          </cell>
-          <cell r="M41">
-            <v>0.20155896000000001</v>
-          </cell>
-          <cell r="N41">
-            <v>36467.272727272728</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42" t="str">
             <v>黑龙江省</v>
           </cell>
-          <cell r="M42">
-            <v>0.2451802218181818</v>
-          </cell>
-          <cell r="N42">
-            <v>30132.545454545456</v>
-          </cell>
         </row>
         <row r="43">
           <cell r="A43" t="str">
             <v>上海市</v>
-          </cell>
-          <cell r="M43">
-            <v>0.36066765818181817</v>
-          </cell>
-          <cell r="N43">
-            <v>82561.454545454544</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44" t="str">
             <v>江苏省</v>
           </cell>
-          <cell r="M44">
-            <v>0.89354548727272731</v>
-          </cell>
-          <cell r="N44">
-            <v>61125.090909090912</v>
-          </cell>
         </row>
         <row r="45">
           <cell r="A45" t="str">
             <v>浙江省</v>
-          </cell>
-          <cell r="M45">
-            <v>0.62796972181818189</v>
-          </cell>
-          <cell r="N45">
-            <v>57482.545454545456</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46" t="str">
             <v>安徽省</v>
           </cell>
-          <cell r="M46">
-            <v>0.31065335363636365</v>
-          </cell>
-          <cell r="N46">
-            <v>24569.272727272728</v>
-          </cell>
         </row>
         <row r="47">
           <cell r="A47" t="str">
             <v>福建省</v>
-          </cell>
-          <cell r="M47">
-            <v>0.36020714636363632</v>
-          </cell>
-          <cell r="N47">
-            <v>46761.909090909088</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48" t="str">
             <v>江西省</v>
           </cell>
-          <cell r="M48">
-            <v>0.22357112909090909</v>
-          </cell>
-          <cell r="N48">
-            <v>25197</v>
-          </cell>
         </row>
         <row r="49">
           <cell r="A49" t="str">
             <v>山东省</v>
-          </cell>
-          <cell r="M49">
-            <v>0.90066113818181814</v>
-          </cell>
-          <cell r="N49">
-            <v>46441.272727272728</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50" t="str">
             <v>河南省</v>
           </cell>
-          <cell r="M50">
-            <v>0.5360834772727272</v>
-          </cell>
-          <cell r="N50">
-            <v>27877.81818181818</v>
-          </cell>
         </row>
         <row r="51">
           <cell r="A51" t="str">
             <v>湖北省</v>
-          </cell>
-          <cell r="M51">
-            <v>0.38928826454545457</v>
-          </cell>
-          <cell r="N51">
-            <v>33548.727272727272</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52" t="str">
             <v>湖南省</v>
           </cell>
-          <cell r="M52">
-            <v>0.3920309881818182</v>
-          </cell>
-          <cell r="N52">
-            <v>29063.909090909092</v>
-          </cell>
         </row>
         <row r="53">
           <cell r="A53" t="str">
             <v>广东省</v>
-          </cell>
-          <cell r="M53">
-            <v>1</v>
-          </cell>
-          <cell r="N53">
-            <v>50171.090909090912</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54" t="str">
             <v>广西壮族自治区</v>
           </cell>
-          <cell r="M54">
-            <v>0.23077194454545455</v>
-          </cell>
-          <cell r="N54">
-            <v>23978.090909090908</v>
-          </cell>
         </row>
         <row r="55">
           <cell r="A55" t="str">
             <v>海南省</v>
-          </cell>
-          <cell r="M55">
-            <v>4.9993580545454545E-2</v>
-          </cell>
-          <cell r="N55">
-            <v>28125.090909090908</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56" t="str">
             <v>重庆市</v>
           </cell>
-          <cell r="M56">
-            <v>0.2009587818181818</v>
-          </cell>
-          <cell r="N56">
-            <v>34125.63636363636</v>
-          </cell>
         </row>
         <row r="57">
           <cell r="A57" t="str">
             <v>四川省</v>
-          </cell>
-          <cell r="M57">
-            <v>0.42294704818181822</v>
-          </cell>
-          <cell r="N57">
-            <v>25253.545454545456</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58" t="str">
             <v>贵州省</v>
           </cell>
-          <cell r="M58">
-            <v>0.1271954509090909</v>
-          </cell>
-          <cell r="N58">
-            <v>17852.454545454544</v>
-          </cell>
         </row>
         <row r="59">
           <cell r="A59" t="str">
             <v>云南省</v>
-          </cell>
-          <cell r="M59">
-            <v>0.18794610272727272</v>
-          </cell>
-          <cell r="N59">
-            <v>21261.454545454544</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60" t="str">
             <v>陕西省</v>
           </cell>
-          <cell r="M60">
-            <v>0.24070429454545453</v>
-          </cell>
-          <cell r="N60">
-            <v>32436.636363636364</v>
-          </cell>
         </row>
         <row r="61">
           <cell r="A61" t="str">
             <v>甘肃省</v>
-          </cell>
-          <cell r="M61">
-            <v>9.783243245454544E-2</v>
-          </cell>
-          <cell r="N61">
-            <v>18865.363636363636</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62" t="str">
             <v>青海省</v>
           </cell>
-          <cell r="M62">
-            <v>3.0233603727272726E-2</v>
-          </cell>
-          <cell r="N62">
-            <v>28389.272727272728</v>
-          </cell>
         </row>
         <row r="63">
           <cell r="A63" t="str">
             <v>宁夏回族自治区</v>
-          </cell>
-          <cell r="M63">
-            <v>3.8591624454545455E-2</v>
-          </cell>
-          <cell r="N63">
-            <v>30641.363636363636</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64" t="str">
             <v>新疆维吾尔自治区</v>
           </cell>
-          <cell r="M64">
-            <v>0.12878631545454544</v>
-          </cell>
-          <cell r="N64">
-            <v>29029.727272727272</v>
-          </cell>
         </row>
         <row r="65">
           <cell r="A65" t="str">
             <v>均值</v>
-          </cell>
-          <cell r="B65">
-            <v>0.32694432643333343</v>
-          </cell>
-          <cell r="C65">
-            <v>0.32777863923333345</v>
-          </cell>
-          <cell r="D65">
-            <v>0.33924597256666672</v>
-          </cell>
-          <cell r="E65">
-            <v>0.33822347569999994</v>
-          </cell>
-          <cell r="F65">
-            <v>0.32331315796666671</v>
-          </cell>
-          <cell r="G65">
-            <v>0.33297034736666675</v>
-          </cell>
-          <cell r="H65">
-            <v>0.34551824716666679</v>
-          </cell>
-          <cell r="I65">
-            <v>0.34614557196666668</v>
-          </cell>
-          <cell r="J65">
-            <v>0.3467888683</v>
-          </cell>
-          <cell r="K65">
-            <v>0.33952300600000007</v>
-          </cell>
-          <cell r="L65">
-            <v>0.3318479473999999</v>
-          </cell>
-          <cell r="M65">
-            <v>0.33620905091818187</v>
-          </cell>
-          <cell r="N65">
-            <v>38729.50909090908</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66" t="str">
-            <v>东部均值</v>
-          </cell>
-          <cell r="B66">
-            <v>0.50763044927272727</v>
-          </cell>
-          <cell r="C66">
-            <v>0.50822203109090913</v>
-          </cell>
-          <cell r="D66">
-            <v>0.5180789369090909</v>
-          </cell>
-          <cell r="E66">
-            <v>0.51766910990909087</v>
-          </cell>
-          <cell r="F66">
-            <v>0.4991410056363636</v>
-          </cell>
-          <cell r="G66">
-            <v>0.5055203310909091</v>
-          </cell>
-          <cell r="H66">
-            <v>0.51736862000000006</v>
-          </cell>
-          <cell r="I66">
-            <v>0.51951328400000019</v>
-          </cell>
-          <cell r="J66">
-            <v>0.51868557545454541</v>
-          </cell>
-          <cell r="K66">
-            <v>0.50925686045454543</v>
-          </cell>
-          <cell r="L66">
-            <v>0.495647224</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67" t="str">
-            <v>中部均值</v>
-          </cell>
-          <cell r="B67">
-            <v>0.28477477999999995</v>
-          </cell>
-          <cell r="C67">
-            <v>0.287620453</v>
-          </cell>
-          <cell r="D67">
-            <v>0.30303295100000005</v>
-          </cell>
-          <cell r="E67">
-            <v>0.30152486099999998</v>
-          </cell>
-          <cell r="F67">
-            <v>0.286065978</v>
-          </cell>
-          <cell r="G67">
-            <v>0.29949611500000001</v>
-          </cell>
-          <cell r="H67">
-            <v>0.31272502899999999</v>
-          </cell>
-          <cell r="I67">
-            <v>0.31024468799999994</v>
-          </cell>
-          <cell r="J67">
-            <v>0.31028450299999999</v>
-          </cell>
-          <cell r="K67">
-            <v>0.30209395900000002</v>
-          </cell>
-          <cell r="L67">
-            <v>0.29591337299999998</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68" t="str">
-            <v>西部均值</v>
-          </cell>
-          <cell r="B68">
-            <v>0.15296078344444441</v>
-          </cell>
-          <cell r="C68">
-            <v>0.15185692277777774</v>
-          </cell>
-          <cell r="D68">
-            <v>0.1609090401111111</v>
-          </cell>
-          <cell r="E68">
-            <v>0.15967727244444443</v>
-          </cell>
-          <cell r="F68">
-            <v>0.1497982107777778</v>
-          </cell>
-          <cell r="G68">
-            <v>0.15926951433333331</v>
-          </cell>
-          <cell r="H68">
-            <v>0.1719158116666667</v>
-          </cell>
-          <cell r="I68">
-            <v>0.17414157277777775</v>
-          </cell>
-          <cell r="J68">
-            <v>0.17725329877777776</v>
-          </cell>
-          <cell r="K68">
-            <v>0.17365834722222223</v>
-          </cell>
-          <cell r="L68">
-            <v>0.17157613644444447</v>
           </cell>
         </row>
       </sheetData>
@@ -7070,14 +6465,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F78" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="W36" workbookViewId="0">
+      <selection activeCell="AK44" sqref="AK44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>